<commit_message>
exp viz analysis fig made
</commit_message>
<xml_diff>
--- a/chapter_3_vpa_mesc_cyst_emb_redo/vpa_only_exp1/results/final_list_for_text/vpa_only_exp1_final_list.xlsx
+++ b/chapter_3_vpa_mesc_cyst_emb_redo/vpa_only_exp1/results/final_list_for_text/vpa_only_exp1_final_list.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dasha\Documents\GitHub\dissertation_related\chapter_3_vpa_mesc_cyst_emb_redo\vpa_only_exp1\results\final_list_for_text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{35BE3E43-F938-474A-AF0A-A9DE667E3299}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9014C2DE-3B44-4FD2-B0DC-FC894229D17A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25170" windowHeight="11085"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25170" windowHeight="11085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vpa_cell_neg_top_hits_w_FC_pval" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
     <t>myo-Inositol</t>
   </si>
   <si>
-    <t>N-alpha-Acetylglutamine</t>
-  </si>
-  <si>
     <t>Asparagine</t>
   </si>
   <si>
@@ -46,21 +43,9 @@
     <t>Deoxyribose</t>
   </si>
   <si>
-    <t>Glycerol 1-phosphoserine</t>
-  </si>
-  <si>
-    <t>G3P</t>
-  </si>
-  <si>
     <t>Glyceric Acid</t>
   </si>
   <si>
-    <t>Sedoheptulose 7-phosphate</t>
-  </si>
-  <si>
-    <t>D-Glucose 6-phosphate</t>
-  </si>
-  <si>
     <t>Succinoadenosine</t>
   </si>
   <si>
@@ -106,9 +91,6 @@
     <t>Homocitric Acid</t>
   </si>
   <si>
-    <t>Valproic acid</t>
-  </si>
-  <si>
     <t>ADP-Glucose</t>
   </si>
   <si>
@@ -184,9 +166,6 @@
     <t>Nicotinamide</t>
   </si>
   <si>
-    <t>D-Ribose</t>
-  </si>
-  <si>
     <t>GlcNAc</t>
   </si>
   <si>
@@ -205,24 +184,15 @@
     <t>Uridine</t>
   </si>
   <si>
-    <t>D-Galactitol</t>
-  </si>
-  <si>
     <t>NMN</t>
   </si>
   <si>
-    <t>Glycerol-3-phosphocholine</t>
-  </si>
-  <si>
     <t>Proline</t>
   </si>
   <si>
     <t>PC(36:4)</t>
   </si>
   <si>
-    <t>Methyl-L-Lysine</t>
-  </si>
-  <si>
     <t>Thiamine</t>
   </si>
   <si>
@@ -230,12 +200,42 @@
   </si>
   <si>
     <t>Media</t>
+  </si>
+  <si>
+    <t>Galactitol</t>
+  </si>
+  <si>
+    <t>Ribose</t>
+  </si>
+  <si>
+    <t>Methyl-Lysine</t>
+  </si>
+  <si>
+    <t>N-Acetylglutamine</t>
+  </si>
+  <si>
+    <t>Glucose 6-Phosphate</t>
+  </si>
+  <si>
+    <t>Glyceraldehyde 3-Phosphate</t>
+  </si>
+  <si>
+    <t>Glycerol 1-Phosphoserine</t>
+  </si>
+  <si>
+    <t>Glycerol-3-Phosphocholine</t>
+  </si>
+  <si>
+    <t>Sedoheptulose 7-Phosphate</t>
+  </si>
+  <si>
+    <t>Valproic Acid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1078,11 +1078,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,36 +1097,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>1.46</v>
@@ -1137,16 +1137,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>1.48</v>
@@ -1157,16 +1157,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>1.53</v>
@@ -1177,13 +1177,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1197,13 +1197,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1217,13 +1217,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1237,16 +1237,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>1.59</v>
@@ -1257,16 +1257,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>1.42</v>
@@ -1277,13 +1277,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -1297,13 +1297,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -1317,13 +1317,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -1337,16 +1337,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>1.44</v>
@@ -1357,16 +1357,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E14">
         <v>1.58</v>
@@ -1377,16 +1377,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E15">
         <v>1.46</v>
@@ -1397,13 +1397,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
@@ -1417,13 +1417,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
@@ -1437,16 +1437,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E18">
         <v>1.51</v>
@@ -1457,16 +1457,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E19">
         <v>1.4</v>
@@ -1477,16 +1477,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E20">
         <v>1.29</v>
@@ -1497,13 +1497,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
@@ -1517,13 +1517,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
@@ -1537,13 +1537,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
@@ -1557,13 +1557,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
@@ -1577,13 +1577,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
         <v>0</v>
@@ -1597,16 +1597,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E26">
         <v>1.53</v>
@@ -1617,13 +1617,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
@@ -1637,13 +1637,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
@@ -1657,13 +1657,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
@@ -1677,13 +1677,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D30" t="s">
         <v>0</v>
@@ -1697,13 +1697,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D31" t="s">
         <v>0</v>
@@ -1717,13 +1717,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
         <v>0</v>
@@ -1737,13 +1737,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
         <v>0</v>
@@ -1757,13 +1757,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D34" t="s">
         <v>0</v>
@@ -1777,13 +1777,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D35" t="s">
         <v>0</v>
@@ -1797,13 +1797,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
         <v>0</v>
@@ -1817,13 +1817,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D37" t="s">
         <v>0</v>
@@ -1837,16 +1837,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D38" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E38">
         <v>1.21</v>
@@ -1857,13 +1857,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
         <v>0</v>
@@ -1877,16 +1877,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E40">
         <v>1.48</v>
@@ -1897,16 +1897,16 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E41">
         <v>1.91</v>
@@ -1917,13 +1917,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D42" t="s">
         <v>0</v>
@@ -1937,13 +1937,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D43" t="s">
         <v>0</v>
@@ -1957,13 +1957,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D44" t="s">
         <v>0</v>
@@ -1977,13 +1977,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D45" t="s">
         <v>0</v>
@@ -1997,16 +1997,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E46">
         <v>1.32</v>
@@ -2020,10 +2020,10 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D47" t="s">
         <v>0</v>
@@ -2040,10 +2040,10 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D48" t="s">
         <v>0</v>
@@ -2057,13 +2057,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C49" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D49" t="s">
         <v>0</v>
@@ -2077,13 +2077,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C50" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D50" t="s">
         <v>0</v>
@@ -2097,13 +2097,13 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D51" t="s">
         <v>0</v>
@@ -2117,13 +2117,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C52" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D52" t="s">
         <v>0</v>
@@ -2137,16 +2137,16 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C53" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D53" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E53">
         <v>1.56</v>
@@ -2157,16 +2157,16 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B54" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C54" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D54" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E54">
         <v>1.35</v>
@@ -2177,16 +2177,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D55" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E55">
         <v>1.21</v>
@@ -2197,16 +2197,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C56" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D56" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E56">
         <v>1.49</v>
@@ -2217,16 +2217,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C57" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D57" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E57">
         <v>1.89</v>
@@ -2237,13 +2237,13 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C58" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D58" t="s">
         <v>0</v>
@@ -2257,13 +2257,13 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C59" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D59" t="s">
         <v>0</v>
@@ -2277,16 +2277,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D60" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E60">
         <v>1.25</v>
@@ -2297,13 +2297,13 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D61" t="s">
         <v>0</v>
@@ -2317,16 +2317,16 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C62" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D62" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E62">
         <v>1.25</v>
@@ -2337,13 +2337,13 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D63" t="s">
         <v>0</v>
@@ -2357,16 +2357,16 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C64" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D64" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E64">
         <v>1.24</v>
@@ -2377,13 +2377,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C65" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D65" t="s">
         <v>0</v>
@@ -2397,13 +2397,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C66" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D66" t="s">
         <v>0</v>
@@ -2417,13 +2417,13 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C67" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D67" t="s">
         <v>0</v>
@@ -2437,13 +2437,13 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C68" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D68" t="s">
         <v>0</v>
@@ -2457,16 +2457,16 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C69" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D69" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E69">
         <v>1.4</v>
@@ -2477,16 +2477,16 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C70" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D70" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E70">
         <v>1.85</v>
@@ -2497,16 +2497,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C71" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D71" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E71">
         <v>35.71</v>
@@ -2520,10 +2520,10 @@
         <v>2</v>
       </c>
       <c r="B72" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C72" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D72" t="s">
         <v>0</v>
@@ -2540,10 +2540,10 @@
         <v>2</v>
       </c>
       <c r="B73" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C73" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D73" t="s">
         <v>0</v>
@@ -2557,13 +2557,13 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C74" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D74" t="s">
         <v>0</v>
@@ -2577,13 +2577,13 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C75" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D75" t="s">
         <v>0</v>

</xml_diff>